<commit_message>
keast fix incorrect vera 1992 pmid
</commit_message>
<xml_diff>
--- a/models/keast-bladder/source/keast-bladder.xlsx
+++ b/models/keast-bladder/source/keast-bladder.xlsx
@@ -4092,7 +4092,7 @@
     <t>L6-S1 sensory neurons innervating bladder</t>
   </si>
   <si>
-    <t>PMID:1619047,PMID:7174880,PMID:4700666,PMID:11382385,PMID:11382385,PMID:32598494</t>
+    <t>PMID:1619047,PMID:7174880,PMID:4700666,PMID:11382385,PMID:1358408,PMID:32598494</t>
   </si>
   <si>
     <t>ilxtr:neuron-type-keast-10</t>
@@ -4107,7 +4107,7 @@
     <t>L1-L2 sensory neurons innervating bladder</t>
   </si>
   <si>
-    <t>PMID:4700666,PMID:11382385,PMID:3558884,PMID:1619047,PMID:2891149,PMID:11382385</t>
+    <t>PMID:4700666,PMID:11382385,PMID:3558884,PMID:1619047,PMID:2891149,PMID:1358408</t>
   </si>
   <si>
     <t>ilxtr:neuron-type-keast-11</t>
@@ -4206,7 +4206,7 @@
     <t>sympathetic chain ganglion neuron OR paravertebral sympathetic ganglion neuron</t>
   </si>
   <si>
-    <t>PMID:11382385,PMID:9622251,PMID:7174880,PMID:9442414</t>
+    <t>PMID:1358408,PMID:9622251,PMID:7174880,PMID:9442414</t>
   </si>
   <si>
     <t>ilxtr:neuron-type-keast-4</t>
@@ -4233,7 +4233,7 @@
     <t>sympathetic preganglionic neuron innervating pelvic ganglion neuron</t>
   </si>
   <si>
-    <t>PMID:11382385,PMID:3225349,PMID:30704972,PMID:3558884,PMID:2891149,PMID:10473279,PMID:21283532,PMID:758335,PMID:1726105</t>
+    <t>PMID:1358408,PMID:3225349,PMID:30704972,PMID:3558884,PMID:2891149,PMID:10473279,PMID:21283532,PMID:758335,PMID:1726105</t>
   </si>
   <si>
     <t>ilxtr:neuron-type-keast-6</t>
@@ -4260,7 +4260,7 @@
     <t>sympathetic preganglionic neuron innervating sympathetic chain ganglion neuron</t>
   </si>
   <si>
-    <t>PMID:11382385,PMID:2891149,PMID:2567744,PMID:1726105</t>
+    <t>PMID:1358408,PMID:2891149,PMID:2567744,PMID:1726105</t>
   </si>
   <si>
     <t>ilxtr:neuron-type-keast-8</t>

</xml_diff>

<commit_message>
kblad resolve some ntk 8 issues
</commit_message>
<xml_diff>
--- a/models/keast-bladder/source/keast-bladder.xlsx
+++ b/models/keast-bladder/source/keast-bladder.xlsx
@@ -2538,16 +2538,16 @@
     <t>T12 sympathetic ganglia SPR axon chain to T13_Neuron 8 (kblad)</t>
   </si>
   <si>
+    <t>ns40</t>
+  </si>
+  <si>
     <t>ns38</t>
   </si>
   <si>
-    <t>ns40</t>
-  </si>
-  <si>
     <t>0,0,0</t>
   </si>
   <si>
-    <t>K78, K70, K79</t>
+    <t>K79, K70, K78</t>
   </si>
   <si>
     <t>ac-sgt13-l1</t>
@@ -2559,7 +2559,7 @@
     <t>ns41</t>
   </si>
   <si>
-    <t>K79, K71, K80</t>
+    <t>K80, K71, K79</t>
   </si>
   <si>
     <t>ac-sgt13-l1join</t>
@@ -2577,7 +2577,7 @@
     <t>ns42</t>
   </si>
   <si>
-    <t>K80, K72, K81</t>
+    <t>K81, K72, K80</t>
   </si>
   <si>
     <t>ac-sgl1-l2join</t>
@@ -2595,7 +2595,7 @@
     <t>ns43</t>
   </si>
   <si>
-    <t>K81, K73, K82</t>
+    <t>K82, K73, K81</t>
   </si>
   <si>
     <t>ac-sgl3-l4</t>
@@ -12957,10 +12957,10 @@
         <v>212</v>
       </c>
       <c r="F31" s="146" t="s">
-        <v>829</v>
+        <v>834</v>
       </c>
       <c r="G31" s="154" t="s">
-        <v>834</v>
+        <v>828</v>
       </c>
       <c r="H31" s="149"/>
       <c r="I31" s="150"/>
@@ -12971,7 +12971,6 @@
       <c r="L31" s="155" t="s">
         <v>835</v>
       </c>
-      <c r="M31" s="155"/>
       <c r="N31" s="155"/>
       <c r="O31" s="153"/>
       <c r="P31" s="153"/>
@@ -12991,10 +12990,10 @@
         <v>212</v>
       </c>
       <c r="F32" s="156" t="s">
+        <v>834</v>
+      </c>
+      <c r="G32" s="154" t="s">
         <v>816</v>
-      </c>
-      <c r="G32" s="154" t="s">
-        <v>834</v>
       </c>
       <c r="H32" s="149"/>
       <c r="I32" s="150"/>
@@ -13025,10 +13024,10 @@
         <v>212</v>
       </c>
       <c r="F33" s="157" t="s">
+        <v>840</v>
+      </c>
+      <c r="G33" s="158" t="s">
         <v>834</v>
-      </c>
-      <c r="G33" s="158" t="s">
-        <v>840</v>
       </c>
       <c r="H33" s="149"/>
       <c r="I33" s="150"/>
@@ -13058,11 +13057,11 @@
       <c r="E34" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="F34" s="159" t="s">
+      <c r="F34" s="158" t="s">
+        <v>840</v>
+      </c>
+      <c r="G34" s="159" t="s">
         <v>824</v>
-      </c>
-      <c r="G34" s="158" t="s">
-        <v>840</v>
       </c>
       <c r="H34" s="149"/>
       <c r="I34" s="150"/>
@@ -13092,11 +13091,11 @@
       <c r="E35" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="F35" s="160" t="s">
+      <c r="F35" s="148" t="s">
+        <v>846</v>
+      </c>
+      <c r="G35" s="160" t="s">
         <v>840</v>
-      </c>
-      <c r="G35" s="148" t="s">
-        <v>846</v>
       </c>
       <c r="H35" s="149"/>
       <c r="I35" s="150"/>
@@ -13141,7 +13140,6 @@
       <c r="L36" s="155" t="s">
         <v>851</v>
       </c>
-      <c r="M36" s="155"/>
       <c r="N36" s="155"/>
       <c r="O36" s="153"/>
       <c r="P36" s="153"/>

</xml_diff>